<commit_message>
worked on research about the companies
</commit_message>
<xml_diff>
--- a/Internship_Search.xlsx
+++ b/Internship_Search.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\internship-search-log-augustosplett\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B5B7D8-31C5-477C-9C9E-5AC5225F9E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC50986-9B37-448C-9D13-BE91C71B7CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12855" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Company Name</t>
   </si>
@@ -139,6 +139,48 @@
   </si>
   <si>
     <t>https://ca.indeed.com/rc/clk?jk=f4331cfef9b85d9b&amp;bb=FiEnwVt6ityTI7xeoewqEwX8hM1Mo3dJpDSzl8dHxBdNMPWS0EJ4TwQF-nLa2rpIE6_KCMuvej2Adevv_y_sEipJGo9PCNCxe2SC8baRzp0kFxUgF_jDPIZmS3x-fiSS&amp;xkcb=SoBP67M37Bv3j9QB3Z0MbzkdCdPP&amp;fccid=e66b3d356c96d114&amp;vjs=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Desjardins Group (French: Mouvement Desjardins) is a Canadian financial service cooperative and the largest federation of credit unions (French: caisses populaires) in North America. It was founded in 1900 in Lévis, Quebec by Alphonse Desjardins.[2] While its legal headquarters remains in Lévis, most of the executive management, including the CEO, is based in Montreal.[3]
+As of 2017, Desjardins Group consists of 293 local credit unions operating 1,032 points of service and serving more than seven million members and clients, mostly in the provinces of Quebec and Ontario.[4] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Société Générale S.A. (French: [sɔsjete ʒeneʁal]), colloquially known in English speaking countries as SocGen (French: [sɔk ʒɛn]),[3] is a French-based multinational financial services company founded in 1864, registered in downtown Paris and headquartered nearby in La Défense.
+Société Générale is France's third largest bank by total assets after BNP Paribas and Crédit Agricole.[4] It is also the sixth largest bank in Europe and the world's eighteenth.[4] It is considered to be a systemically important bank by the Financial Stability Board. It has been designated as a Significant Institution since the entry into force of European Banking Supervision in late 2014, and as a consequence is directly supervised by the European Central Bank.[5][6]
+From 1966 to 2003 it was known as one of the Trois Vieilles ("Old Three") major French commercial banks, along with Banque Nationale de Paris (from 2000 BNP Paribas) and Crédit Lyonnais. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrox Graphics, Inc. is a producer of video card components and equipment for personal computers and workstations. Based in Dorval, Quebec, Canada, it was founded in 1976 by Lorne Trottier and Branko Matić. The name is derived from "Ma" in Matić and "Tro" in Trottier.[2] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Caisse de dépôt et placement du Québec (CDPQ) est un investisseur institutionnel gérant notamment le régime de rentes du Québec et plusieurs autres régimes de retraite et d’assurances publics et parapublics du Québec.
+Elle a été créée par le gouvernement de Jean Lesage le 15 juillet 1965 par une loi du Parlement du Québec. Il s'agit du deuxième plus important fonds de pension au Canada, après le Régime de pensions du Canada1. Au 30 juin 2023, la CDPQ gère un actif net de 434 milliards de dollars canadiens investi au Canada et à l’étranger2. Son siège social est situé à Québec, dans l'Édifice Price et le bureau d'affaires principal est situé à Montréal, dans l'Édifice Jacques-Parizeau. </t>
+  </si>
+  <si>
+    <t>A cooperative platform to bring together Canada's restaurants, couriers and food lovers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IAMGOLD is an intermediate gold producer and developer based in Canada with operating mines in North America and West Africa. The Company has commenced production at the large-scale, long life Côté Gold Mine in partnership with Sumitomo Metal Mining Co. Ltd., which is expected to be among the largest gold mines in Canada. In addition, the Company has an established portfolio of early stage and advanced exploration projects within high potential mining districts. IAMGOLD employs approximately 3,600 people and is committed to maintaining its culture of accountable mining through high standards of Environmental, Social and Governance practices, including its commitment to Zero Harm®, in every aspect of its business. IAMGOLD is listed on the New York Stock Exchange (NYSE:IAG) and the Toronto Stock Exchange (TSX:IMG) and is one of the companies on the Jantzi Social Index, a socially screened market capitalization-weighted consisting of companies which pass a set of broadly based environmental, social and governance rating criteria. </t>
+  </si>
+  <si>
+    <t>Intact Financial Corporation is a Canadian multinational property and casualty insurance company. Originally established in 1809 as the Halifax Fire Insurance Association, it was later acquired by Nationale-Nederlanden; from 1993 to 2009, it was a subsidiary of the Dutch multinational ING Group under the name ING Canada. Intact Financial directly underwrites insurance through its subsidiary companies Intact Insurance and Belair Insurance (operating as Belairdirect), as well as operating additional brokerage, insurance service, and damage restoration subsidiaries. As of 2017, Intact was the largest provider of property and casualty insurance in Canada by annual premiums.
+The company has over 16,000 employees and insures more than five million individuals and businesses through its insurance subsidiaries. In the J.D. Power 2015 Canadian Home Insurance Satisfaction Study, belairdirect was ranked highest in the Atlantic/Ontario region with a score of 799 and in the Quebec region with a score of 814 and Intact Insurance ranked third with a score of 791.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caterpillar Inc., also known as Cat, is an American construction, mining and other engineering equipment manufacturer.[6] The company is the world's largest manufacturer of construction equipment.[3][7][8] In 2018, Caterpillar was ranked number 73 on the Fortune 500 list[9] and number 265 on the Global Fortune 500 list.[10] Caterpillar stock is a component of the Dow Jones Industrial Average.[11]
+Caterpillar Inc. traces its origins to the 1925 merger of the Holt Manufacturing Company and the C. L. Best Tractor Company, creating a new entity, California-based Caterpillar Tractor Company.[12] In 1986, the company reorganized itself as a Delaware corporation under the current name, Caterpillar Inc. It announced in January 2017 that over the course of that year, it would relocate its headquarters from Peoria, Illinois, to Deerfield, Illinois, scrapping plans from 2015 of building an $800 million new headquarters complex in downtown Peoria.[13][14] Its headquarters are located in Irving, Texas, since 2022.[15][16]
+The company also licenses and markets a line of clothing and workwear boots under its Cat / Caterpillar name.[17][18] Additionally, the company licenses the Cat phone brand of toughened mobile phones and rugged smartphones since 2012.[19] Caterpillar machinery and other company-branded products are recognizable by their trademark "Caterpillar Yellow" livery and the "CAT" logo.[20] </t>
+  </si>
+  <si>
+    <t>Workland is a company that specializes in personalized recruitment technologies, solutions and services. After spending many years recruiting and co-developing technologies in partnership with its customers from both the private and public sector, Workland has developed unique expertise in both technologies and services.</t>
+  </si>
+  <si>
+    <t>The art gallery of old Montreal presents local artists from Montreal, focused on street art paintings for sale and contemporary art as well as interior and exterior murals. Our contemporary art gallery in Saint-Paul has been open since 2020 and positions itself as a committed art gallery with works driven by a political will. From abstract to surrealism via pop culture, the paintings represent the spectrum of urban art. The Quebec painters of our gallery of art in old Montreal contrasts with the usually older art galleries of Saint-Paul. We display the pioneers of street art and have at heart the local Quebec artists who create our murals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Notre mission est de remédier à la disparité économique chronique dans les communautés d'ascendance africaine. Grâce à de nouvelles technologies et à des initiatives innovantes, nous visons à favoriser des modèles durables de prospérité pour les enjeux particuliers qui touchent spécifiquement l'aspect socio-économique de nos communautés. Ensemble, en travaillant ensemble, nous nous efforçons de nous connecter pour atteindre un objectif: UP - Unir et Prospérer.  
+Orijin est une organisation à but non lucratif dédiée au développement économique des personnes d'ascendance africaine ainsi qu'au renforcement de leur rôle économique, financier et social grâce à la technologie et à de nouveaux modèles d'acquisition et de distribution de richesse. Orijin cherche à lutter contre les inégalités économiques chroniques dans les communautés d'ascendance africaine. Nous voulons encourager les personnes ciblées à investir dans leur santé économique en achetant et en consommant dans des entreprises d'ascendance africaine.</t>
   </si>
 </sst>
 </file>
@@ -232,7 +274,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8378327F-677A-482F-ADA7-0B01547DCBB9}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8378327F-677A-482F-ADA7-0B01547DCBB9}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E12" xr:uid="{8378327F-677A-482F-ADA7-0B01547DCBB9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -241,11 +283,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C4B65219-A5EC-449C-A66B-90D043A36744}" name="Company Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B28E6B72-D0BB-4CB2-8517-5769A5BE30F8}" name="About the Company" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{02D99432-F306-41AD-BD4A-43F765A6C3D3}" name="Position" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{7CC27DCD-2695-448C-BA28-EBB43B353BFD}" name="URL" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2922B726-4E01-4B0C-8C9B-85716BB16084}" name="Possible Point of Contact" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C4B65219-A5EC-449C-A66B-90D043A36744}" name="Company Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B28E6B72-D0BB-4CB2-8517-5769A5BE30F8}" name="About the Company" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{02D99432-F306-41AD-BD4A-43F765A6C3D3}" name="Position" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7CC27DCD-2695-448C-BA28-EBB43B353BFD}" name="URL" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{2922B726-4E01-4B0C-8C9B-85716BB16084}" name="Possible Point of Contact" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -516,20 +558,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="17.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.62890625" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.3671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="79" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5234375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,10 +589,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -557,10 +603,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -568,10 +617,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
@@ -579,9 +631,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -594,6 +649,9 @@
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
@@ -601,10 +659,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
@@ -612,10 +673,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
@@ -623,10 +687,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
@@ -634,10 +701,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
@@ -645,10 +715,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -656,9 +729,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="331.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>35</v>

</xml_diff>